<commit_message>
instructions change 3 and 4
</commit_message>
<xml_diff>
--- a/new_instructions_3.xlsx
+++ b/new_instructions_3.xlsx
@@ -17,7 +17,7 @@
     <t>instruct_text</t>
   </si>
   <si>
-    <t xml:space="preserve">You'll be given a blank textbox under the image, where you can type out all the details of the story you can remember. </t>
+    <t xml:space="preserve">You'll be given a blank text box under the image, where you can type out all the details of the story you can remember. </t>
   </si>
   <si>
     <t xml:space="preserve">There is a 5 minute time limit for recalling each story. </t>
@@ -275,7 +275,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="bottom" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -290,7 +290,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment vertical="bottom" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -1425,13 +1425,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
     <col min="8" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>